<commit_message>
Entrega Final Miry Carpeta de Trabajo Toyota
</commit_message>
<xml_diff>
--- a/TOYOTA-Celaya/Fuentes - Toyota/Distribuidor/Servicios/Citas - Telemarketing/Toyota - CEL - Analisis - Servicio - Citas_CRT - v1_1_1 - Parte CRT No Implementada Formalmente.xlsx
+++ b/TOYOTA-Celaya/Fuentes - Toyota/Distribuidor/Servicios/Citas - Telemarketing/Toyota - CEL - Analisis - Servicio - Citas_CRT - v1_1_1 - Parte CRT No Implementada Formalmente.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KE\JMM\PROCESSES MAPPING\toyota_proceso\TOYOTA-Celaya\Fuentes - Toyota\Distribuidor\Servicios\Citas - Telemarketing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C0928C-797D-4E1E-8053-0EBDA50E15D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E5B5110-6D1D-4DD1-81B6-44FFDC3FA96A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="255" yWindow="225" windowWidth="19950" windowHeight="10590" activeTab="1" xr2:uid="{7E74557B-02A4-44EF-8F45-FC026D5565D6}"/>
+    <workbookView xWindow="330" yWindow="105" windowWidth="19950" windowHeight="10590" activeTab="1" xr2:uid="{7E74557B-02A4-44EF-8F45-FC026D5565D6}"/>
   </bookViews>
   <sheets>
     <sheet name="FTO Task List" sheetId="4" r:id="rId1"/>
@@ -1648,9 +1648,6 @@
     <t>Una opcion para Visualizar las Campañas Activas de un Modelo asociado a un Cliente, incluida Descripcion.</t>
   </si>
   <si>
-    <t>Numeros Telenicos</t>
-  </si>
-  <si>
     <t>Se solicita que los Numeros Telefonicos sean de 10 Digitos. Analizar Alcance, Toyota si les envia un Reporte donde identica estos datos como Incorrectos.</t>
   </si>
   <si>
@@ -1736,12 +1733,15 @@
   <si>
     <t>Para modalidad de recoleccion del Auto del Cliente. Se puede Homologar un Esquema de Datos Alternativos que se usen para SERV Movil y Recoleccion de acuerdo al Tipo de Servicio / Orden.</t>
   </si>
+  <si>
+    <t>Numeros Telefonicos</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1865,6 +1865,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2016,7 +2023,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2146,6 +2153,9 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2761,7 +2771,7 @@
       </c>
       <c r="Y5" s="34"/>
       <c r="Z5" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AA5" s="5" t="s">
         <v>128</v>
@@ -2830,11 +2840,11 @@
       </c>
       <c r="Y6" s="34"/>
       <c r="Z6" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AA6" s="5"/>
       <c r="AB6" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="7" spans="2:28" ht="75" x14ac:dyDescent="0.25">
@@ -3201,7 +3211,7 @@
       <c r="AA12" s="5"/>
       <c r="AB12" s="7"/>
     </row>
-    <row r="13" spans="2:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:28" ht="135" x14ac:dyDescent="0.25">
       <c r="B13" s="32" t="s">
         <v>17</v>
       </c>
@@ -3260,7 +3270,7 @@
       <c r="AA13" s="5"/>
       <c r="AB13" s="7"/>
     </row>
-    <row r="14" spans="2:28" ht="135" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:28" ht="120" x14ac:dyDescent="0.25">
       <c r="B14" s="32" t="s">
         <v>17</v>
       </c>
@@ -3319,7 +3329,7 @@
       <c r="AA14" s="5"/>
       <c r="AB14" s="7"/>
     </row>
-    <row r="15" spans="2:28" ht="90" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:28" ht="75" x14ac:dyDescent="0.25">
       <c r="B15" s="32" t="s">
         <v>17</v>
       </c>
@@ -4993,9 +5003,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4862388-C0C2-40EF-9FDF-90ED8985F146}">
   <dimension ref="B2:X41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5328,33 +5338,33 @@
       <c r="W8" s="23"/>
     </row>
     <row r="9" spans="2:23" ht="60" x14ac:dyDescent="0.25">
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="44" t="s">
+        <v>334</v>
+      </c>
+      <c r="C9" s="44" t="s">
+        <v>319</v>
+      </c>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44" t="s">
+        <v>308</v>
+      </c>
+      <c r="F9" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="44" t="s">
         <v>324</v>
       </c>
-      <c r="C9" s="22" t="s">
-        <v>319</v>
-      </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22" t="s">
-        <v>308</v>
-      </c>
-      <c r="F9" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="22" t="s">
-        <v>325</v>
-      </c>
-      <c r="I9" s="22" t="s">
+      <c r="I9" s="44" t="s">
         <v>312</v>
       </c>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22" t="s">
+      <c r="J9" s="44"/>
+      <c r="K9" s="44" t="s">
         <v>304</v>
       </c>
-      <c r="L9" s="22" t="s">
+      <c r="L9" s="44" t="s">
         <v>20</v>
       </c>
       <c r="M9" s="22"/>
@@ -5375,7 +5385,7 @@
     </row>
     <row r="10" spans="2:23" ht="75" x14ac:dyDescent="0.25">
       <c r="B10" s="22" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C10" s="22" t="s">
         <v>86</v>
@@ -5391,14 +5401,14 @@
         <v>15</v>
       </c>
       <c r="H10" s="22" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I10" s="22" t="s">
         <v>312</v>
       </c>
       <c r="J10" s="22"/>
       <c r="K10" s="22" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="L10" s="22"/>
       <c r="M10" s="22"/>
@@ -5419,7 +5429,7 @@
     </row>
     <row r="11" spans="2:23" ht="60" x14ac:dyDescent="0.25">
       <c r="B11" s="22" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C11" s="22" t="s">
         <v>86</v>
@@ -5435,14 +5445,14 @@
         <v>15</v>
       </c>
       <c r="H11" s="22" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="I11" s="22" t="s">
         <v>312</v>
       </c>
       <c r="J11" s="22"/>
       <c r="K11" s="22" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="L11" s="22"/>
       <c r="M11" s="22"/>
@@ -5463,7 +5473,7 @@
     </row>
     <row r="12" spans="2:23" ht="60" x14ac:dyDescent="0.25">
       <c r="B12" s="22" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C12" s="22" t="s">
         <v>314</v>
@@ -5479,14 +5489,14 @@
         <v>15</v>
       </c>
       <c r="H12" s="22" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="I12" s="22" t="s">
         <v>312</v>
       </c>
       <c r="J12" s="22"/>
       <c r="K12" s="22" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="L12" s="22"/>
       <c r="M12" s="22"/>
@@ -5507,7 +5517,7 @@
     </row>
     <row r="13" spans="2:23" ht="60" x14ac:dyDescent="0.25">
       <c r="B13" s="22" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C13" s="22" t="s">
         <v>316</v>
@@ -5523,14 +5533,14 @@
         <v>15</v>
       </c>
       <c r="H13" s="22" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="I13" s="22" t="s">
         <v>312</v>
       </c>
       <c r="J13" s="22"/>
       <c r="K13" s="22" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="L13" s="22"/>
       <c r="M13" s="22"/>

</xml_diff>